<commit_message>
small changes to run code
</commit_message>
<xml_diff>
--- a/market_research.xlsx
+++ b/market_research.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,335 +584,672 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc.</t>
+          <t>MagnaChip Semiconductor Corporation</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MLNK</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc. is a company that specializes in providing technology solutions for financial institutions, particularly focusing on consumer lending. Here are some key points regarding MeridianLink's business based on the provided information:
-1. **Product Expansion**: MeridianLink focuses on continuous product innovation to help customers succeed in serving consumers. They have introduced new products like MeridianLink Engage, which helps financial institutions increase engagement and profitability through data-driven lending campaigns. Additionally, they have acquired StreetShares to expand their small business lending offerings to banks and credit unions【4:0†source】【4:1†source】.
-2. **Financial Performance**: The company has shown strong financial performance, with GAAP revenue up 7% year over year in the first quarter of 2022. They have a usage-based SaaS recurring revenue model, with a significant portion of revenue coming from subscription fees. MeridianLink's gross margin was 66% in Q1, and they continue to invest in sales, marketing, and R&amp;D efforts to drive organic growth【4:0†source】【4:2†source】.
-3. **Market Positioning**: MeridianLink is outperforming in the market due to their diversified portfolio of products offered in an integrated platform and the strong digitalization trends. They are making investments in services capacity to convert more bookings to revenue and focusing on development in the cloud to enhance and expand their product suite. The company is positioned to drive further growth through M&amp;A, expansion of the partner marketplace, and organic product development【4:2†source】.
-4. **Guidance and Outlook**: Despite fluctuations in the mortgage market, MeridianLink remains confident in their momentum and has a robust pipeline. The company expects continued growth in revenue and adjusted EBITDA margins for the full year of 2022. They are increasing investments to accelerate implementation capacity and bring recurring revenue online more quickly【4:3†source】【4:4†source】.
-In summary, MeridianLink Inc. is a technology company specializing in financial solutions, showing consistent growth, strong financial performance, and a strategic focus on innovation and market positioning to drive future success in the financial technology industry.</t>
+          <t>### Business Description of MagnaChip Semiconductor Corporation
+MagnaChip Semiconductor Corporation is a company based in South Korea, listed on the NYSE under the ticker symbol MX. They are a designer and manufacturer of analog and mixed-signal semiconductor platform solutions for various applications including communication, Internet of Things (IoT), consumer, computing, industrial, and automotive sectors. With over 45 years of operating history, MagnaChip owns a significant portfolio of approximately 1,000 registered patents and pending applications, showcasing extensive expertise in engineering, design, and manufacturing processes. The company offers a wide range of standard products to customers globally.
+Financially, MagnaChip reported strong performance in their recent quarterly earnings reports. In Q3 2024, the company achieved high revenue at the upper end of guidance, driven by growth in their Standard Product businesses, which include MSS and PAS segments. Sequentially, Standard Product revenue increased by 25.9%, with notable growth in the discrete Power business due to leaner inventory and new product design wins. The CEO highlighted increased demand for products targeting China smartphones, automotive displays, and OLED IT. Looking ahead, MagnaChip expects a modest sequential decline in Standard Product business revenue in Q4 but reiterates full-year guidance for double-digit growth in both MSS and PAS businesses in 2024.
+In Q2 2024, MagnaChip also performed well, with revenue above the mid-point of guidance and better-than-expected gross margin. The Standard Products Business saw double-digit sequential revenue growth, supported by recovery in the Power business, increased demand for OLED drivers, and growth in Power IC demand for OLED IT panels and LED TVs. The company anticipates further sequential revenue growth in the Standard Product Business in Q3.
+MagnaChip faces risks typical of the semiconductor industry, such as competitive products and pricing, manufacturing capacity constraints, supply chain disruptions, and macroeconomic conditions. They aim to address these challenges while leveraging their technological expertise and diverse product offerings to sustain growth and profitability.
+For further details, refer to the full reports on MagnaChip Semiconductor Corporation's financial performance and operational highlights from the Business Wire articles linked below:
+1. [Q3 2024 Earnings Report](https://www.businesswire.com/news/home/20241030615593/en/Magnachip-Reports-Results-for-Third-Quarter-2024) 
+2. [Q2 2024 Earnings Report](https://www.businesswire.com/news/home/20240731545229/en/Magnachip-Reports-Results-for-Second-Quarter-2024) 
+For additional information, you can visit MagnaChip's website at www.magnachip.com. 
+---
+These insights were extracted from the financial reports provided by Business Wire. For more detailed information, you may refer to the original source documents.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc. offers lending software solutions and data verification software solutions. Here is a breakdown of their main products and services based on the information provided:
-1. **Lending Software Solutions**:
-   - These solutions accounted for nearly 68% of MeridianLink's total revenue and experienced a 14% year-over-year growth in revenue.
-   - Specific products under lending software solutions include LoansPQ, LendingQB, XpressAccounts, AchievEngine, and XpressCollect.
-   - The revenue from these solutions grew 19% year over year, excluding the impact from the anticipated slowdown in mortgage-related revenues.
-2. **Data Verification Software Solutions**:
-   - Revenue from data verification software solutions decreased by 4% year over year due to a decline in mortgage-related revenues.
-   - These solutions are focused on providing data verification services tied to mortgage activities.
-3. **Mortgage Market**:
-   - In the first quarter, revenues from the mortgage loan market generated 28% of MeridianLink's overall revenues, with 7% of lending software solution revenues and 70% of data verification software solutions revenues tied to mortgage-focused products.
-   - The company's data verification software solutions outperformed the market by continuously adding value through additional data items and partnerships to enhance customer offerings.
-MeridianLink's products and services aim to streamline lending and account origination processes for banks, credit unions, and financial institutions, empowering them to scale efficiently and support their compliance efforts while delivering an enhanced experience for both staff and consumers【4:0†source】.</t>
+          <t>MagnaChip Semiconductor Corporation is a designer and manufacturer of analog and mixed-signal semiconductor platform solutions. The company provides a broad range of standard products to customers worldwide. Their main product categories include:
+1. **Standard Products Business**:
+   - This includes **Mixed-Signal Solutions (MSS)** and **Power Analog Solutions (PAS)**, which showed significant sequential growth in revenue according to their financial reports【4:0†source】【4:1†source】.
+2. **Transitional Fab 3 Foundry Services**:
+   - Transitional Fab 3 foundry services are also part of MagnaChip's offerings, contributing to their total revenues【4:3†source】【4:4†source】.
+These products cater to applications in communication, Internet of Things (IoT), consumer electronics, computing, industrial, and automotive sectors. Additionally, MagnaChip has a long operating history, owns a significant portfolio of patents, and has expertise in engineering, design, and manufacturing processes【4:2†source】.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc.'s primary target market or industry vertical is the Financial Services industry, with a focus on banks, credit unions, mortgage lenders, specialty lending providers, and consumer reporting agencies【4:0†source】【4:1†source】.</t>
+          <t>MagnaChip Semiconductor Corporation's primary target market or industry vertical includes communication, Internet of Things (IoT), consumer, computing, industrial, and automotive applications. They offer a broad range of standard products to customers worldwide in these sectors【4:0†source】. Specifically, they have been focusing on mobile applications such as smartphones, battery protection, and quick chargers, aiming to grow their presence in this market by targeting global smartphone OEMs and ODMs【4:1†source】.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc.'s secondary target market includes institutions smaller than their typical customer size, which they have enabled to win through a wholly templatized implementation. These contracts are smaller in value compared to their typical customers but further extend their market-leading capabilities to institutions of all sizes committed to providing top capabilities in the market【4:1†source】.</t>
+          <t>MagnaChip Semiconductor Corporation's secondary target market is in Brazil, where they have created a new business unit focused on batteries for smartphones. Additionally, they are planning to target other areas in Brazil, including communications devices such as Wi-Fi, Bluetooth modules, and other products to support the Internet of Things (IoT) markets【4:1†source】.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc.'s tertiary target market includes mid-market financial institutions that aim to serve their clients better, outperform competitors, and enhance their efficiency through better access to data and faster decision-making in their businesses for their clients. MeridianLink offers a platform that enables these institutions to run a significant portion of their business operations efficiently, engage with a broader customer base, and improve risk analysis to offer competitive rates【4:0†source】.</t>
+          <t>MagnaChip Semiconductor Corporation's tertiary target market includes areas in Brazil such as communications devices like Wi-Fi, Bluetooth modules, and other products supporting the Internet of Things (IoT) markets. Additionally, the company is focused on developing batteries for smartphones in Brazil as part of its strategic market expansion plans【4:1†source】.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc. primarily serves the Financial Services and Banking industries. The largest segments of its customers are in Financial Services (37%) and Banking (35%). Furthermore, 96% of MeridianLink customers are based in the United States【4:4†source】.</t>
+          <t>MagnaChip Semiconductor Corporation serves significant markets such as communication, Internet of Things (IoT), consumer, computing, industrial, and automotive applications with its analog and mixed-signal semiconductor platform solutions【4:2†source】.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>The total addressable market size for MeridianLink Inc.'s primary market can be estimated based on its revenue figures. In the first quarter, MeridianLink generated total revenue of $72.8 million, with 87% coming from subscription fees【4:1†source】. Since subscription fees are a recurring revenue stream in the SaaS model, we can consider this portion of the revenue as reflective of the market size available to MeridianLink within its primary market. 
-By calculating 87% of the total revenue, we find that approximately $63.36 million of the total revenue represents the addressable market size for MeridianLink Inc.'s primary market in the first quarter. This figure gives an indication of the scale of the market opportunity for MeridianLink within its primary market segment.</t>
+          <t>The total addressable market size for MagnaChip Semiconductor Corporation's primary market is not explicitly mentioned in the provided documents. To determine this figure, additional market research focusing on the semiconductor industry, MagnaChip's product offerings, target customer segments, and geographical reach would be necessary. For a more detailed analysis, it may be beneficial to consult industry reports, market research databases, and company presentations or disclosures.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>The total addressable market size for MeridianLink Inc.'s secondary market is not explicitly provided in the provided documents. Further market research or financial analysis specific to MeridianLink Inc. or the secondary market segment would be needed to determine the total addressable market size.</t>
+          <t>The estimated total addressable market size for MagnaChip Semiconductor Corporation's secondary market is around $500 million to $600 million【4:1†source】.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>The total addressable market size for MeridianLink Inc.'s tertiary market is not directly available in the searched documents. To determine the specific total addressable market size for MeridianLink Inc.'s tertiary market, additional information or market research specific to their tertiary market segment would be needed. If you have access to additional data or reports focusing on MeridianLink Inc.'s tertiary market, that would be instrumental in determining the total addressable market size for that segment.</t>
+          <t>The total addressable market size for MagnaChip Semiconductor Corporation's tertiary market is estimated to be around $500 million to $600 million, with the aim to capture their fair share of this market .</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>The total addressable market size (in USD) for MeridianLink Inc.'s other significant markets is not explicitly provided in the documents available. To determine this figure, additional sources such as market research reports or company disclosures specifically detailing the TAM for MeridianLink Inc.'s other significant markets would be necessary.</t>
+          <t>To determine the total addressable market size for MagnaChip Semiconductor Corporation's other significant markets, we would need to gather specific information on the revenue breakdown by market segment and the estimated market sizes for each segment. Unfortunately, the documents provided do not contain direct information on the total addressable market size for MagnaChip Semiconductor Corporation's other significant markets.
+For a detailed analysis of MagnaChip Semiconductor Corporation's total addressable market size in its significant markets, additional sources such as market research reports, industry analyses, or company disclosures specifically detailing market segment revenues and estimates would be necessary.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for MeridianLink Inc.'s primary market is expected to be 9.52% from today's value【4:0†source】.</t>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for MagnaChip Semiconductor Corporation's primary market is expected to be 24.37% by 2025【4:0†source】.</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>The projected 5-year compound annual growth rate (CAGR) for MeridianLink Inc.'s secondary market is expected to be around 9.52%【4:1†source】.</t>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for MagnaChip Semiconductor Corporation's secondary market is estimated to be 24.37% by the year 2025【4:0†source】.</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>The projected 5-year CAGR for MeridianLink Inc.'s tertiary market is not explicitly provided in the documents available. However, there are forecasts indicating price ranges and potential returns for the company's stock over different time frames, highlighting varying trends and outlooks for investors【4:0†source】【4:1†source】【4:2†source】【4:4†source】.</t>
+          <t>The projected 5-year CAGR for MagnaChip Semiconductor Corporation's tertiary market is not explicitly mentioned in the provided documents. The information primarily focuses on price forecasts, market sentiment, and revenue growth percentages over various periods. For specific details on the 5-year CAGR for MagnaChip Semiconductor Corporation's tertiary market, additional data or sources may be required outside of the uploaded documents【4:0†source】【4:1†source】【4:2†source】【4:3†source】【4:4†source】.</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>The projected 5-year CAGR for MeridianLink Inc.'s other markets is not explicitly mentioned in the provided documents. The information mainly focuses on stock price predictions and market trends, but does not specifically address the projected 5-year CAGR for other markets of MeridianLink Inc.【4:0†source】【4:1†source】【4:2†source】【4:3†source】. For a detailed analysis of the projected 5-year CAGR for MeridianLink Inc.'s other markets, additional information may be required.</t>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for MagnaChip Semiconductor Corporation's other markets indicates an increase in prices potentially reaching $5.61 by 2025, representing a 24.37% gain from today's value. However, for the year 2030, the stock is forecasted to be priced between $1.557834 and $2.44. Overall, the long-term forecast for MagnaChip Semiconductor suggests a bearish trend with potential highs of $5.61 and lows of $0.800248 over the period【4:0†source】.</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>**Competitive Analysis of MeridianLink Inc.:**
-**Strengths:**
-1. **Diversified Product Portfolio:** MeridianLink offers a comprehensive, consolidated cloud platform supporting consumer loan and account types, including mortgage, which contributes to outperforming in the market【4:1†source】.
-2. **Market-leading Offering:** MeridianLink resonates with a market segment seeking to serve clients better and outperform competitors, positioning the company as a market leader with broad integrations, platform breadth, and capability acceleration【4:4†source】.
-3. **Strong Momentum in Business Segments:** The company has shown notable strength in the consumer lending side of the business with strong momentum and continued investment in go-to-market strategies, resulting in new logo wins and cross-sell opportunities【4:1†source】.
-**Weaknesses:**
-1. **Revenue Dependency on Mortgage Sector:** While experiencing strong growth, MeridianLink's revenue is impacted by the mortgage sector, comprising approximately 27% of revenues in Q4. The company expects this percentage to decrease due to expected weakening mortgage volumes, highlighting revenue concentration in this area【4:1†source】.
-2. **Limited Increase in ARR on New Logo Sales:** The company indicated that there isn't a noticeable increase in Annual Recurring Revenue (ARR) on new logo sales. This suggests a potential challenge in maximizing revenue growth from new customers, although pruning smaller customer bases may lead to a higher ARR per customer【4:3†source】.
-In conclusion, MeridianLink Inc. benefits from a diversified product portfolio and a strong market position appealing to customers seeking enhanced digital solutions. However, revenue dependency on the mortgage sector and limited growth in ARR from new customers are areas of vulnerability that the company may need to address for sustained competitiveness.</t>
+          <t>### MagnaChip Semiconductor Corporation: Competitive Analysis
+#### Strengths:
+1. **Growth Potential:** MagnaChip Semiconductor reported a surge in gross profit margin, reaching the highest level in the company's history, despite limited sales growth【4:0†source】.
+2. **Product Diversification:** MagnaChip operates in the semiconductor sector, offering a range of solutions including display parts for TVs and other consumer electronics【4:4†source】.
+#### Weaknesses:
+1. **Sales Performance:** Sales for MagnaChip Semiconductor only increased by 1.8% year over year in Q3 2021, with display solutions sales notably weak, falling nearly 16% year over year due to supply chain constraints【4:0†source】.
+2. **Supply Constraints:** Management expects supply constraints to persist, limiting revenue growth potential and impacting the company's ability to capitalize on strong gross margins【4:0†source】.
+#### Market Position:
+1. **Competitors:** Competitors of MagnaChip Semiconductor include companies like Canadian Solar, Nano Dimension, Navitas Semiconductor, and others in the electronic equipment industry【4:2†source】.
+2. **Strategic Positioning:** MagnaChip has become a buyout target, with rumors of buyout offers from entities like LX Group and Carlyle Group, indicating potential interest in the company amidst industry challenges【4:4†source】.
+In conclusion, MagnaChip Semiconductor Corporation exhibits strengths in its profit margin growth and product diversification, but faces challenges in sales growth and supply constraints. Understanding and mitigating these weaknesses while leveraging its competitive strengths will be crucial for its future market positioning.</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc. has an estimated market share of about 7.6% in the Loan Management category, which includes loan originating software, digital lending platforms, and digital banking technology【4:1†source】.</t>
+          <t>To determine MagnaChip Semiconductor Corporation's current estimated market share percentage in their primary market, we need to analyze their performance and compare it to competitors. Unfortunately, the documents provided did not contain specific information about MagnaChip's exact market share percentage. However, based on competitor analysis, some of their competitors in the electronic equipment industry include Canadian Solar, Nano Dimension, Navitas Semiconductor, and others【4:4†source】. 
+To obtain the most up-to-date market share percentage for MagnaChip Semiconductor Corporation, I recommend checking industry reports, market research websites, or financial news sources that specialize in semiconductor market analysis. This will provide you with the latest data on MagnaChip's market share and positioning within the industry.</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Based on the available information, MeridianLink Inc. currently holds a market share of about 7.6% in the Loan Management category. Looking ahead, the company is projected to see a price increase, potentially reaching between $12.57 and $21.06 by 2025【4:1†source】. However, it is important to note that this information does not directly provide a specific projected market share percentage for MeridianLink Inc. in 5 years. For a more precise estimation of the projected market share percentage, additional data or forecasts specific to market share would be needed.</t>
+          <t>Based on the analysis, MagnaChip Semiconductor Corporation is projected to have a stock price between $4.03 and $5.61 by 2025. This represents a potential gain of 24.37% from the current value【4:3†source】. However, there is no specific information available regarding the projected market share percentage for MagnaChip Semiconductor Corporation in 5 years.</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc. has a market share of about 7.6% in the Loan Management category. The main competitors of MeridianLink include companies like Q2, Kanzhun, Freshworks, and Intapp among others in the computer software industry. Comparatively, Q2 is reported to beat MeridianLink on 11 of the 17 factors compared between the two stocks【4:0†source】【4:1†source】【4:3†source】.</t>
+          <t>MagnaChip Semiconductor Corporation's main competitors include Canadian Solar, Nano Dimension, Navitas Semiconductor, BlackSky Technology, nLIGHT, Canaan, Varex Imaging, Clearfield, SkyWater Technology, and Gilat Satellite Networks within the electronic equipment industry. Among these competitors, Canadian Solar outperforms MagnaChip Semiconductor on 12 out of 17 factors compared between the two stocks【4:2†source】.</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc. operates in the competitive landscape alongside key competitors such as Q2, Kanzhun, Freshworks, Intapp, Workiva, SoundHound AI, Science Applications International, Tenable, Varonis Systems, and Cellebrite DI within the computer software industry【4:1†source】. MeridianLink differentiates itself by offering a platform that enables financial institutions to run a large portion of their business, resonating particularly with mid-market financial institutions that aim to outperform competitors. The company's integrated platform, breadth of products, and focus on accelerating mid-market financial institutions position it as a market leader within the industry【4:4†source】.
-MeridianLink's competitive strategy involves continued investments in its go-to-market organization, expansion beyond its sales sweet spot, innovative product suite integration and modernization, and reducing implementation times to drive faster go-lives. The company's strong go-to-market engine has led to record bookings, new logo wins, and accelerated cross-selling, indicating a robust growth trajectory. By focusing on providing comprehensive and efficient solutions, MeridianLink aims to meet the evolving needs of financial institutions in a post-COVID world characterized by increased digitalization and competition【4:3†source】.</t>
+          <t>MagnaChip Semiconductor Corporation operates in the electronic equipment industry and faces competition from companies such as Canadian Solar, Nano Dimension, Navitas Semiconductor, and others. In comparison to Canadian Solar, MagnaChip Semiconductor lags behind on various factors, with Canadian Solar outperforming MagnaChip on 12 out of 17 compared aspects【4:0†source】. 
+In terms of stock performance and market positioning, MagnaChip Semiconductor has faced challenges related to declining sales in Q1 2022 due to supply chain issues, a situation not unique to the company within the semiconductor industry. Despite these challenges, institutional investors still see value in MagnaChip, considering that the stock trades for less than 13 times trailing 12-month earnings. Additionally, with semiconductor demand expected to rise in the coming years, there are opportunities for companies like MagnaChip, even amidst market concerns【4:2†source】. 
+Overall, while facing competitive pressures and market challenges, MagnaChip Semiconductor Corporation remains a player in the semiconductor industry with potential for growth and value, supported by its product offerings and market positioning.</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc.'s primary industry classification is within the "computer software" industry, as indicated by its main competitors including Q2, Kanzhun, Freshworks, and others in the same industry【4:0†source】.</t>
+          <t>MagnaChip Semiconductor Corporation is primarily classified in the semiconductor industry, specifically as a designer and manufacturer of analog and mixed-signal semiconductor platform solutions for various applications such as communication, Internet of Things (IoT), consumer, computing, industrial, and automotive sectors【4:0†source】.</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc.'s industry sub-classification is within the "computer software" industry【4:1†source】.</t>
+          <t>MagnaChip Semiconductor Corporation is classified as a designer and manufacturer of analog and mixed-signal semiconductor platform solutions for various applications such as communication, Internet of Things (IoT), consumer electronics, computing, industrial, and automotive sectors【4:0†source】【4:2†source】.</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc. operates primarily in the Financial Services industry. The company's products and services include loan originating software, digital lending platforms, and digital banking technology aimed at helping banks, credit unions, and financial institutions streamline their lending and account origination processes【4:0†source】.</t>
+          <t>The detailed industry category of MagnaChip Semiconductor Corporation is as follows: They are a designer and manufacturer of analog and mixed-signal semiconductor platform solutions for communication, Internet of Things (IoT), consumer, computing, industrial, and automotive applications, providing a broad range of standard products to customers worldwide 【4:2†source】.</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>The most appropriate SIC code for MeridianLink Inc. would likely fall under the category of 7372 - Prepackaged Software. This classification typically includes companies that develop and publish software packages for mass distribution to end-users. The activities of MeridianLink Inc., such as providing lending software solutions, align well with this SIC code category【4:1†source】.</t>
+          <t>The most appropriate SIC code for MagnaChip Semiconductor Corporation, a designer and manufacturer of analog and mixed-signal semiconductor platform solutions, would likely fall under the SIC code 3674, which corresponds to Semiconductors and Related Devices【4:0†source】.</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>The most appropriate NAICS code for MeridianLink Inc. based on the information provided is likely 511210, which corresponds to "Software Publishers". This code aligns with the fact that MeridianLink Inc. is involved in providing software solutions, particularly lending software solutions【4:1†source】.</t>
+          <t>The most appropriate NAICS code for MagnaChip Semiconductor Corporation is 334413, which corresponds to "Semiconductor and Related Device Manufacturing"【4:0†source】.</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc.'s industry is classified as part of the "computer software" industry on LinkedIn【4:1†source】.</t>
+          <t>MagnaChip Semiconductor Corporation's industry classification on LinkedIn is not explicitly mentioned in the documents provided. However, according to information from MarketBeat, MagnaChip Semiconductor Corporation and its main competitors like Canadian Solar, Nano Dimension, Navitas Semiconductor, and others are all part of the "electronic equipment" industry【4:3†source】.</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>MeridianLink Inc. is primarily classified within the "Financial Services" industry based on the companies that use MeridianLink's products. Additionally, looking at the data related to MeridianLink's market share and customer industry segments, it is evident that the company mainly serves the Financial Services and Banking sectors, with the majority of its customers being medium-sized businesses in the United States【4:0†source】【4:2†source】.</t>
+          <t>Relevant industry classifications for MagnaChip Semiconductor Corporation include being part of the "electronic equipment" industry. Some of its main competitors in this industry are Canadian Solar, Nano Dimension, Navitas Semiconductor, and others【4:1†source】.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PagerDuty Inc.</t>
+          <t>SMART Global Holdings Inc.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PD</t>
+          <t>SGH</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PagerDuty Inc. is a global leader in digital operations management, providing customers with a comprehensive platform to manage real-time incident responses and optimize workflows. The company focuses on enterprise and mid-market clients, with a growth strategy centered around expansion and new product developments, including integrating AI capabilities into its offerings. PagerDuty emphasizes substantial investment in product innovation to ensure competitiveness and adaptability. In Q3 of fiscal 2025, PagerDuty achieved a 9.4% year-over-year revenue increase to $118.9 million, with notable growth in operating income and recognition as an AI Operations leader. Despite challenges such as an operating loss and a decline in dollar-based net retention rate, the company remains optimistic about its fiscal trajectory and is committed to sustaining growth through strategic initiatives like integrating AI, expanding internationally, and enhancing customer retention【4:1†source】【4:2†source】.</t>
+          <t>SMART Global Holdings Inc. recently faced challenges with disappointing quarterly results and weak forward guidance, leading to a significant decrease in stock price. The company reported a decline in net sales and missed earnings expectations for the fiscal fourth quarter, partly due to divesting its Smart Brazil operations. Despite these setbacks, the company aims to transform into an enterprise solutions company focused on improving gross margins and higher quality revenue. SMART Global Holdings is focusing on its high-margin services sector, with a successful increase in service revenue and enhanced customer engagements. However, revenue decreased notably in the first quarter of fiscal year 2024, driven by reductions in several segments. The company also highlighted challenges in high-performance computing (HPC) and AI markets, volatile memory pricing, and reduced enterprise spending affecting its financial performance outlook【4:0†source】【4:2†source】.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PagerDuty Inc. offers a range of products and services in the digital operations management space through its PagerDuty Operations Cloud. Some of the main products and services provided by PagerDuty include:
-1. **PagerDuty Operations Cloud**:
-    - Combines AIOps, Automation, Customer Service Operations, and Incident Management.
-    - Utilizes generative AI assistant for flexible, resilient, and scalable operations management.
-2. **Key Features**:
-    - Helps achieve operational efficiency at scale.
-    - Enables automation of end-to-end incident response processes.
-    - Supports businesses in increasing innovation velocity, reducing costs, and mitigating operational risks【4:3†source】.
-PagerDuty's focus is primarily on digital operations management and providing solutions for critical event management use cases. These offerings aim to streamline incident response processes, enhance automation, and improve operational efficiency for businesses of varying sizes and industries.</t>
+          <t>SMART Global Holdings Inc. offers a range of products and services across different business segments:
+1. **Memory Solutions**:
+   - Products include DDR3 DRAM devices.
+   - Services involve supply chain services.
+2. **Intelligent Platform Solutions**:
+   - Products and services offered through the acquisition of Penguin Computing.
+   - Specialty compute and storage solutions targeting applications in artificial intelligence, machine learning, and high-performance computing.
+   - Focus on open technologies and advanced architectures.
+3. **LED Solutions**:
+   - LED products and related services.
+4. **New Business Initiatives**:
+   - Launch of a new business unit in Brazil focusing on battery assembly for smartphones.
+   - Partnership with Samsung SDI for local manufacturing.
+SMART Global Holdings aims to provide high-performance, high-availability enterprise solutions by leveraging its technical expertise, custom design engineering, and commitment to quality across its computing, memory, and LED lines of business【4:0†source】.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>PagerDuty Inc.'s primary target market or industry vertical is focused on enterprise and mid-market clients in the digital operations management space. They empower organizations to manage real-time incident responses and optimize workflows through their comprehensive digital operations management platform【4:0†source】.</t>
+          <t>SMART Global Holdings Inc. primarily focuses on serving its customers through high-performance, high-availability enterprise solutions in the computing, memory, and LED sectors. The company emphasizes providing deep technical knowledge, custom design engineering, build-to-order flexibility, and a commitment to top-quality products across these business lines【4:2†source】.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>PagerDuty Inc.'s secondary target market is focused on addressing technical operations, business continuity, and use cases in infrastructure, making it a suitable alternative for critical event management use cases【4:2†source】.</t>
+          <t>The secondary target market of SMART Global Holdings Inc. is not directly mentioned in the provided documents. For more specific information on SMART Global Holdings Inc.'s secondary target market, additional sources or company disclosures focusing on their market segmentation strategy would be needed.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>PagerDuty Inc.'s tertiary target market includes focusing on enterprise and mid-market clients. PagerDuty's growth strategy revolves around expansion and new product developments, particularly integrating AI capabilities into its offerings【4:1†source】.</t>
+          <t>The tertiary target market for SMART Global Holdings Inc. is not explicitly mentioned in the provided document. For more detailed information on SMART Global Holdings Inc.'s tertiary target market, additional specific market research or company reports may be required.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>PagerDuty Inc. serves significant markets beyond DevOps and SRE. The company focuses on addressing technical operations, business continuity, and infrastructure-related use cases. Additionally, PagerDuty competes in the critical event management space and serves as a suitable alternative for solutions related to incident management, outage resolution, and incident response. Some notable markets PagerDuty serves include AIOps solutions, IT infrastructure monitoring, incident management tools, and AI-powered features for digital operations management【4:0†source】.</t>
+          <t>SMART Global Holdings Inc. serves significant markets in Memory Solutions, Intelligent Platform Solutions, and LED Solutions. These include areas such as high-performance computing, specialty memory solutions, AI, and high-performance computing solutions for enterprise customers【4:0†source】【4:1†source】【4:3†source】.</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>To determine the total addressable market size for PagerDuty Inc.'s primary market, we can use the information related to the company's revenues. In the provided data for PagerDuty Inc., the total net revenues reported for the three months ended September 30, 2024, were $80,369,000. This includes revenues from subscription fees, professional services, and other sources【4:0†source】.
-To estimate the total addressable market size, we would typically consider the market share of PagerDuty Inc. within its primary market and use this to extrapolate the total addressable market size. However, without explicit market share data, a precise calculation cannot be provided. If additional data on market share or specific market segmentation is available, a more accurate estimation could be conducted.</t>
+          <t>The total addressable market size for SMART Global Holdings Inc.'s primary market is not directly provided in the documents searched. To determine this figure, it would be necessary to assess the market size of the specific industry or industries in which SMART Global Holdings operates and then estimate the portion of that market that the company can potentially capture.
+If you have more specific information about the company's primary market or industry, I can help you analyze that data to estimate the total addressable market size.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>To determine the total addressable market size for PagerDuty Inc.'s secondary market, we need to analyze the company's revenue breakdown. From the data provided, PagerDuty's net revenues by major source for the three months ended September 30, 2024, were $80,369,000. The net revenues by solution type for the same period were $80,369,000, with lending software solutions accounting for $63,005,000 and data verification software solutions for $17,364,000【4:0†source】.
-To estimate the total addressable market size for PagerDuty Inc.'s secondary market, we can consider the proportion of revenue attributed to data verification software solutions, which is relevant to the secondary market. In this case, data verification software solutions generated approximately 21.6% of the total net revenue ($17,364,000 out of $80,369,000). Using this percentage, we can estimate the total addressable market size for PagerDuty Inc.'s secondary market at around $17,364,000 / 21.6% = approximately $80,322,222【4:0†source】.</t>
+          <t>The total addressable market size for SMART Global Holdings Inc.'s secondary market is projected to be around $500 million to $600 million【4:3†source】.</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>The total addressable market size for PagerDuty Inc.'s tertiary market is not directly provided in the available documents. If you have access to additional information or specific details about the tertiary market segment of PagerDuty Inc., please provide it for a more accurate analysis.</t>
+          <t>The total addressable market size for SMART Global Holdings Inc.'s tertiary market, specifically the batteries business segment, is estimated to be around a couple of hundred million dollars currently, with around 60% local content regulations in place【4:3†source】.</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>The total addressable market size for PagerDuty Inc.'s other significant markets is not directly available in the documents provided. To determine this information, additional sources specific to PagerDuty's market segmentation and total addressable market for other significant markets would be needed. If you have any other specific queries or need further assistance, please let me know.</t>
+          <t>The total addressable market size for SMART Global Holdings Inc.'s other significant markets is not directly provided in the documents available. Further analysis or specific data related to the total addressable market for SMART Global Holdings Inc.'s different markets would be needed to determine this information.</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>The forecast for PagerDuty Inc. suggests a projected decline over the next several years, with prices potentially reaching $19.05 by 2025. The long-term forecast indicates a bearish trend with potential highs of $19.05 and lows of $2.30 over the period【4:2†source】. However, the specific 5-year CAGR projection for PagerDuty Inc.'s primary market was not explicitly mentioned in the available information. To obtain a precise 5-year CAGR projection for PagerDuty Inc.'s primary market, it may be necessary to consult additional sources or market research reports directly related to the company's financial forecasts.</t>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for SMART Global Holdings Inc.'s primary market is expected to be around 29.94%【4:0†source】.</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>The projected 5-year CAGR for PagerDuty Inc.'s secondary market shows a potential return on investment of -0.94% compared to the current rates by 2025【4:1†source】.</t>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for SMART Global Holdings Inc.'s secondary market is expected to be around 50.62%, with prices potentially reaching $31.40 by 2026【4:0†source】.</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>The projected 5-year CAGR for PagerDuty Inc.'s tertiary market is not explicitly mentioned in the provided documents. For further details on PagerDuty Inc.'s tertiary market growth projection, additional sources or specific reports focusing on this aspect may be needed【4:0†source】.</t>
+          <t>The projected 5-year CAGR for SMART Global Holdings Inc.'s tertiary market is not explicitly provided in the available information. The forecasts cover price predictions, potential returns on investment, and average prices for specific years, but a specific CAGR for the tertiary market over the next 5 years is not mentioned in the data provided【4:0†source】【4:1†source】【4:4†source】.</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>The projected 5-year CAGR for PagerDuty Inc.'s other markets is not directly provided in the available document. If you have additional sources or specific data related to this projection, please provide them for further analysis.</t>
+          <t>The projected 5-year CAGR for SMART Global Holdings Inc.'s other markets is not explicitly mentioned in the available documents. The forecasts mainly focus on stock price predictions and financial performance metrics rather than specific CAGR projections for individual markets. It appears that the documents provide insights into stock price movements, company financials, and general market forecasts rather than detailed market-specific growth rate projections. For more detailed information on the projected 5-year CAGR for SMART Global Holdings Inc.'s other markets, it may be necessary to consult additional sources or reports that specifically address market growth projections for the company's different segments.</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>PagerDuty Inc. demonstrates several competitive strengths and weaknesses in the market:
+          <t>Based on the analysis of SMART Global Holdings Inc., here are some insights into the company's competitive strengths and weaknesses in the market:
+### Competitive Strengths:
+1. **Significant Growth in High-Margin Services Sector:** SMART Global Holdings Inc. has demonstrated significant growth in its high-margin services sector, with service revenue increasing from $31 million to $60 million, constituting 17% of overall sales【4:0†source】.
+2. **Record Non-GAAP Gross Margins:** The company's non-GAAP gross margins reached a record 31.7% for FY23, reflecting an improvement from 29.2% in FY22, indicating successful efforts in enhancing customer engagements【4:0†source】.
+3. **Operational Efficiency:** SMART Global Holdings Inc. has shown operational efficiency with strong cash flow from operating activities totaling $38 million in the fourth quarter, highlighting positive financial performance【4:0†source】.
+### Competitive Weaknesses:
+1. **Substantial Decrease in Revenue:** The company reported a substantial decrease in revenue for the first quarter of fiscal year 2024, with a 13.2% sequential decline and a 29.2% year-over-year decrease, mainly driven by decreases in its Specialty Memory and Intelligent Platform Solutions segments【4:0†source】.
+2. **High Inventory Levels and Weak Demand:** Despite some inventory reduction, elevated levels suggest weak demand and potential oversupply issues, particularly as key customers maintain high inventory levels【4:0†source】.
+3. **Challenges in High-Performance Computing and AI Markets:** Lowered visibility in the high-performance computing and AI markets, along with pressures from volatile memory pricing and diminished enterprise spending, contribute to a deteriorating financial outlook for SMART Global Holdings Inc.【4:0†source】.
+These insights provide a balanced view of SMART Global Holdings Inc.'s market positioning, outlining both strengths and weaknesses that can impact its competitive standing.</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>The current estimated market share percentage of SMART Global Holdings Inc. in their primary market is not explicitly provided in the documents available. To obtain precise market share data, it may be necessary to refer to industry reports, market research publications, or company disclosures specifically addressing this metric.</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>The projected stock forecast for SMART Global Holdings Inc. indicates potential growth over the next few years. By 2026, there is an estimated 50.62% gain from the current value, with prices potentially reaching $31.40. However, the long-term forecast suggests a bearish trend, with highs projected at $31.40 and lows at $9.55. Achieving a specific market share percentage would require further detailed market analysis beyond the provided financial forecast information【4:2†source】.</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>SMART Global Holdings Inc. is positioned as the top company among its peers based on market capitalization, with a Market Cap of $1.103 billion, which is higher than its competitors' market caps【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>SMART Global Holdings Inc.'s competitive position relative to key competitors can be assessed based on recent performance indicators. 
+1. **Financial Performance**:
+   - SMART Global Holdings Inc. reported a substantial decrease in revenue for the first quarter of fiscal year 2024, with a 13.2% sequential decline and a 29.2% year-over-year decrease, mainly driven by decreases in its Specialty Memory and Intelligent Platform Solutions segments. This might indicate challenges in certain segments of its business【4:0†source】.
+   - The company's non-GAAP gross margins reached a record 31.7% for FY23, showcasing a focus on enhancing customer engagements. Additionally, the company demonstrated significant growth in its high-margin services sector, with service revenue increasing from $31 million to $60 million, constituting 17% of overall sales【4:0†source】.
+2. **Future Outlook**:
+   - Smart Global's outlook for financial performance has been affected by lowered visibility in the high-performance computing (HPC) and AI markets, along with pressures from volatile memory pricing and diminished enterprise spending【4:0†source】.
+   - Guidance for Smart Global's first quarter of fiscal 2024 suggests revenue expectations of $250 million to $300 million, with adjusted earnings ranging from breakeven to $0.15 per share, significantly below Wall Street's consensus estimates【4:1†source】.
+3. **Competitive Positioning**:
+   - In comparison to competitors like nLIGHT and X-FAB Silicon Foundries SE, SMART Global Holdings Inc. demonstrates higher total revenue, although it also has higher total debt. It has a market cap larger than nLIGHT, but smaller than X-FAB Silicon Foundries SE. However, its net income is lower compared to these competitors【4:2†source】.
+These insights suggest that while SMART Global Holdings Inc. has shown growth in certain sectors and maintained solid gross margins, it faces challenges and pressure points that impact its revenue and financial outlook. Understanding these dynamics is crucial for evaluating its competitive position in the market.</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>SMART Global Holdings Inc.'s primary industry classification is in the technology sector, specifically focusing on enterprise solutions including computing, memory, and LED products【4:2†source】.</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>SMART Global Holdings Inc. is classified in the Technology sector according to the data provided【4:0†source】.</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>SMART Global Holdings Inc.'s detailed industry category is Technology【4:2†source】.</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>The most appropriate SIC code for SMART Global Holdings, Inc. is 3674, which corresponds to "Semiconductors and Related Devices"【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>The most appropriate NAICS code for SMART Global Holdings Inc. would likely be **334413** which corresponds to "Semiconductor and Related Device Manufacturing" based on the company's sector and business activities in the technology industry【4:2†source】.</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>SMART Global Holdings Inc.'s industry is classified as Technology on LinkedIn【4:0†source】.</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Based on the information available, other relevant industry classifications that apply to SMART Global Holdings Inc. include Technology. SMART Global Holdings is positioned in the Technology sector, focusing on computing, memory, and LED solutions to serve customers with technical knowledge, custom design engineering, flexibility in manufacturing, and a commitment to quality【4:0†source】【4:2†source】.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>LASR</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>**nLIGHT, Inc Business Description:**
+nLIGHT, Inc is a leading provider of high-power semiconductor and fiber lasers for various markets including industrial, microfabrication, and aerospace and defense applications. The company is headquartered in Camas, Washington, and employs over 900 people with operations in the United States, China, Finland, Korea, and Italy. nLIGHT's lasers are instrumental in transforming manufacturing processes and expanding the possibilities of what can be created in these industries【4:4†source】.
+Based on the financial reports, nLIGHT has shown significant performance and growth in its key markets:
+- nLIGHT reported revenues of $56.1 million for the third quarter of 2024, with a substantial increase of 11% compared to the same period in 2023. The company indicated that this growth was largely driven by record results in the Aerospace &amp; Defense sector along with strong performance in Microfabrication【4:0†source】.
+- In the second quarter of 2024, nLIGHT achieved revenues of $50.5 million, showing a 13% increase compared to the first quarter of the same year. The growth in the Aerospace &amp; Defense sector was particularly notable, with a 26% quarter-over-quarter increase. nLIGHT also established a strategic partnership with EOS, a leader in additive manufacturing, positioning the company for further growth in this market【4:3†source】.
+Overall, nLIGHT's focus on high-power semiconductor and fiber lasers for critical sectors like aerospace and defense, combined with strategic partnerships and continuous innovation, underscores the company's commitment to driving growth and leading innovation in its target markets.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc. is a leading provider of high-power semiconductor and fiber lasers for industrial, microfabrication, aerospace, and defense applications. They offer a range of products and services including:
+1. **High-Power Semiconductor Lasers**: Used in various applications such as industrial processes, microfabrication, and defense.
+2. **Fiber Lasers**: Utilized in industrial, microfabrication, aerospace, and defense sectors.
+3. **Aerospace and Defense Products**: nLIGHT provides laser solutions specifically designed for aerospace and defense applications, contributing to record results in this sector【4:0†source】【4:2†source】.
+4. **Microfabrication Applications**: Their lasers are employed in microfabrication processes, showcasing strong execution across multiple programs in the sector【4:2†source】.
+5. **New Product Offerings**: nLIGHT's portfolio expansion includes products like the STACK PACK and STACK Switch products, which are part of the next generation of center-element LED lay-in lights for commercial indoor spaces. Additionally, they introduced the CLAIRITY link in controls as part of their nLight lighting controls platform, offering remote connectivity capability【4:2†source】.
+6. **Intelligent Spaces Group (ISG) Solutions**: nLIGHT's ISG division focuses on leveraging technology to solve problems in spaces, making them smarter, safer, and more environmentally friendly. This involves collecting data through hardware like the Distech controller and analyzing it with software applications powered by Atrius【4:2†source】.
+Overall, nLIGHT's product and service offerings cater to a diverse range of industries including industrial manufacturing, microfabrication, aerospace, defense, and intelligent spaces solutions.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc's primary target market or industry vertical includes aerospace and defense, industrial, and microfabrication applications. They are a leading provider of high-power semiconductor and fiber lasers for these industries【4:0†source】.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc's secondary target market is in the industrial sector. In 2020, their industrial business grew by 10% year-over-year, with continued demand growth in China and opportunities in metal additive manufacturing with their newly introduced AFX 1000 single-mode programmable laser. They focus on providing differentiated programmable laser technology to global industrial customers operating at lower power levels【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc's tertiary target market is not explicitly mentioned in the provided documents. However, based on the information available, nLIGHT primarily focuses on the aerospace and defense, industrial, and microfabrication markets【4:0†source】.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc serves significant markets beyond aerospace and defense, industrial, and microfabrication. They also operate in other geographic regions, with revenue growth in all geographies. In China, their revenue grew by 10% year-over-year in 2020, and sales to customers outside of China grew by 35% year-over-year. Additionally, in the fourth quarter of the same year, they recorded sales outside of China growing by 70% year-over-year, representing 72% of total revenue. This indicates a strong presence and growth in markets outside of China as well【4:0†source】【4:4†source】.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>To determine the total addressable market size for nLIGHT, Inc's primary market, we need specific data related to the market segment served by nLIGHT. The documents provided offer details about nLIGHT's financials, revenue, and operations, but the exact total addressable market size in USD for its primary market is not explicitly mentioned in the available content.
+To calculate the total addressable market size, it would be necessary to gather information on the specific industry or market segment nLIGHT serves and then conduct market research to estimate the total addressable market size within that sector based on factors like market demand, growth projections, and competitor analysis.
+If you have additional information or specific industry details related to nLIGHT's primary market, please provide those to facilitate a more accurate estimation of the total addressable market size.</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>The total addressable market size for nLIGHT, Inc's secondary market is not directly provided in the documents available. For a detailed analysis of the total addressable market size for nLIGHT, Inc's secondary market, additional market research or financial reports specific to the company's market segment would be required.</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>The total addressable market size (in USD) for nLIGHT, Inc's tertiary market is not directly available in the documents provided. For specific details on nLIGHT, Inc's tertiary market size, additional information or market research specific to that segment may be needed.</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To determine the total addressable market size for nLIGHT, Inc's other significant markets, we need to analyze the information provided in the documents. However, the search results did not directly provide the specific total addressable market size in USD for nLIGHT, Inc's other significant markets. 
+To accurately assess the total addressable market size for nLIGHT, Inc's other significant markets, detailed market research on each specific sector and geographical area would be necessary to estimate the potential market size and identify the opportunities available within those segments. This would involve evaluating factors such as target customers, competition, market trends, and the company's positioning within each market.
+For a comprehensive analysis of nLIGHT, Inc's total addressable market size in its other significant markets, a customized market research study focusing on each market individually would be most effective.
+</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>The projected 5-year CAGR for nLIGHT, Inc's primary market is expected to be greater than 20% according to analysts' projections. This growth is forecasted to be at a double-digit annual pace for several years, with a specific mention of a growth rate of 25% over the next few years【4:0†source】.</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for nLIGHT, Inc's secondary market is not explicitly mentioned in the available documents. However, analysts expect significant earnings growth for nLIGHT in the coming years, with consensus projections foreseeing a substantial increase in profits per share annually【4:4†source】.</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Based on the information available, Needham &amp; Co believes that nLIGHT, Inc can generate 25% growth over the next several years with steadily improving profitability in its tertiary market【4:0†source】. This suggests a projected 5-year Compound Annual Growth Rate (CAGR) of 25% for nLIGHT, Inc in its tertiary market.</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>The projected 5-year compound annual growth rate (CAGR) for nLIGHT, Inc in its other markets is expected to be 25%, according to analyst projections. This growth is driven by differentiated technology that is anticipated to lead to steady profitability improvement over the next several years【4:3†source】.</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc is positioned as a strong player in its market with the following competitive strengths and weaknesses based on the information provided:
 **Competitive Strengths:**
-1. **Product Innovation:** PagerDuty invests significantly in product innovation to ensure its platform remains competitive and adaptable, with a focus on integrating AI capabilities into its offerings.
-2. **Financial Performance:** The company achieved a 9.4% year-over-year revenue uplift, reaching $118.9 million, and improved operating income with effective cost management, showcasing financial strength【4:0†source】.
-3. **Market Recognition:** PagerDuty has been recognized as an AI Operations leader by GigaOm, underscoring its innovative AI-powered features and solidifying its position in a competitive market【4:0†source】.
+1. **Technological Differentiation:** nLIGHT is highlighted for its technological differentiation and significant margin leverage potential through vertical integration, which is seen as a reason to invest in the stock【4:4†source】.
+2. **Growth Potential:** Analysts project above-average growth for nLIGHT, with expectations of double-digit annual pace growth for several years, significant margin leverage potential, and a debt-adjusted valuation of about four times annual sales【4:4†source】.
+3. **Industry Recognition:** With a market capitalization of $1 billion, nLIGHT is considered an emerging player in the laser industry, set to generate growth and profitability through differentiated technology【4:1†source】.
 **Competitive Weaknesses:**
-1. **Net Retention Rate Decline:** PagerDuty faced a decline in its dollar-based net retention rate from 110% to 107%, indicating potential challenges in upsell activities【4:0†source】.
-2. **Challenges in Customer Retention:** Despite positive financial results, challenges in customer retention exist, highlighting the need for improved service offerings to enhance customer retention【4:0†source】.
-PagerDuty's strategic focus on product innovation and market recognition are key strengths that contribute to its competitiveness, while challenges related to retention rates and upsell activities represent areas for improvement to maintain market position and sustain growth.</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>PagerDuty Inc.'s current estimated market share percentage in their primary market is not explicitly provided in the available documents. However, you can assess their market positioning and competitiveness by considering their revenue growth, customer base expansion, product innovations, and financial performance detailed in the reports provided【4:0†source】【4:1†source】. If you require a specific market share percentage, it may be necessary to consult additional sources or market research reports.</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>The projected market share percentage for PagerDuty Inc. in 5 years is uncertain based on the available information. However, the company is focused on expanding its enterprise footprint and new product developments to drive growth and innovation in the digital operations management space【4:4†source】. It would be advisable to monitor PagerDuty's market performance and strategic moves over the coming years to assess its potential market share percentage.</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>PagerDuty Inc. is positioned below its main competitor Q2 based on a comparison of various factors. Q2 beats PagerDuty on 13 out of 18 factors considered between the two companies【4:0†source】. Therefore, PagerDuty Inc.'s competitive ranking among its peers is below Q2.</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>PagerDuty Inc. faces competition from several key competitors in the computer software industry. Some notable competitors include:
-1. **Q2 (QTWO)**: Competes with PagerDuty in the computer and technology sector, surpassing PagerDuty in 13 out of 18 factors compared between the two stocks【4:1†source】.
-2. **Freshworks (FRSH)**: Another competitor in the computer software industry challenging PagerDuty's market position【4:1†source】.
-3. **Datadog**: A significant alternative to PagerDuty, offering monitoring, security, and analytics platforms for IT teams. Datadog is crucial for cloud applications and combines infrastructure monitoring, application performance monitoring, and log management, enabling real-time visibility into technology stacks for businesses of all sizes and industries【4:3†source】.
-4. **Better Upti**me: Provides incident management, status pages, and uptime monitoring, with features like advanced team management tools, integrations with Google Calendar, Microsoft Teams, and Slack, and unlimited SMS and phone call alerts on paid plans. It offers a comprehensive solution similar to PagerDuty【4:3†source】.
-5. **ServiceNow IT Service Management**: Simplifies handling service requests and managing IT incidents, offering a centralized incident management system with comprehensive reporting and analytics capabilities. It is a prominent alternative to PagerDuty【4:3†source】.
-6. **Splunk On-Call (formerly VictorOps)**: A cloud-based help desk solution enabling businesses to manage on-call schedules, resolve incidents, and provide visibility into IT infrastructure performance. It offers features for alerts, notifications, chat, activity dashboards, and integration with third-party programs like JIRA, Zendesk, and Slack【4:3†source】.
-PagerDuty Inc. needs to leverage its strengths and unique value propositions to stay competitive in the market against these key competitors.</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>PagerDuty Inc.'s primary industry classification is in the "computer software" industry【4:3†source】.</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>PagerDuty Inc.'s industry sub-classification is within the "computer software" industry, as indicated in a report comparing PagerDuty and its competitors【4:2†source】.</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>PagerDuty Inc.'s detailed industry category is digital operations management. PagerDuty is a global leader in digital operations management, offering a comprehensive platform for managing real-time incident responses and optimizing workflows, with a focus on enterprise and mid-market clients【4:1†source】.</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>The most appropriate SIC code for PagerDuty Inc. would likely fall under the category of "Computer Programming, Data Processing, and Other Computer Related Services," which corresponds to SIC code 7372【4:2†source】.</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>The most appropriate NAICS code for PagerDuty Inc. would likely fall under NAICS code 511210, which is for "Software Publishers" since PagerDuty is a global leader in digital operations management【4:4†source】.</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>PagerDuty Inc.'s industry is classified as part of the "computer software" industry on LinkedIn【4:2†source】.</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>The relevant industry classifications that apply to PagerDuty Inc. include being part of the "computer software" industry【4:1†source】.</t>
+1. **Financial Performance:** nLIGHT faced challenges related to lower overall product revenue and execution issues in its industrial markets. This led to a shortfall in revenue expectations and below-guidance gross margin and Adjusted EBITDA【4:4†source】.
+2. **Profitability Concerns:** Despite being an established company with nearly $140 million in annual sales, nLIGHT currently lacks significant profits and free cash flow, selling at a relatively high multiple of earnings【4:1†source】.
+In conclusion, nLIGHT, Inc stands out for its technological differentiation, growth potential, and industry recognition. However, the company faces challenges in financial performance and profitability which may impact its market competitiveness. Strengthening these areas could further enhance its position in the market.</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>The current estimated market share percentage of nLIGHT, Inc in their primary market is not explicitly provided in the documents available. For a detailed breakdown of nLIGHT's financial performance, market positioning, and comparison with competitors, further market research or reports specifically addressing nLIGHT's market share would be necessary. You may consider consulting industry reports, market analysis studies, or company-specific market share reports to obtain this information.</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>The projected market share percentage for nLIGHT, Inc in 5 years is not explicitly mentioned in the available documents. However, analysts have positive outlooks on nLIGHT, with expectations of significant growth and improved profitability over the next several years. Some projections indicate potential for 25% growth and 50% earnings growth in the near term, with analysts setting target prices that could imply a market cap increase to about $1.3 billion within the next 12 months【4:2†source】【4:4†source】.</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc's competitive ranking among its peers is superior to Planet Labs PBC according to MarketBeat's analysis【4:3†source】.</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc competes in the electronic equipment industry with key competitors including Planet Labs PBC, Silicon Motion Technology, Himax Technologies, and others. In a comparison with Planet Labs PBC, nLIGHT outperforms on various factors such as community ranking, valuation, risk, institutional ownership, dividends, profitability, analyst recommendations, and earnings【4:0†source】.
+Analysts view nLIGHT as an emerging player with strong growth potential thanks to its technological differentiation and significant margin leverage potential through vertical integration. Despite being smaller in market capitalization compared to some competitors like IPG Photonics, nLIGHT is expected to achieve double-digit annual growth and improved profitability, with optimistic projections for sales and earnings growth. Analysts have provided target price ranges for nLIGHT stock, indicating potential market cap growth in the near future【4:1†source】.
+Overall, nLIGHT's competitive position seems strong with a focus on technology differentiation, margin expansion potential, and a positive growth outlook, positioning the company well against its key competitors in the industry.</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc.'s primary industry classification is as a leading provider of high-power semiconductor and fiber lasers for aerospace and defense, industrial, and microfabrication applications【4:2†source】.</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc operates in the "electronic equipment" industry along with competitors like Planet Labs PBC, Silicon Motion Technology, Himax Technologies, and others【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc is detailed as a leading provider of high-power semiconductor and fiber lasers for aerospace and defense, industrial, and microfabrication applications【4:3†source】.</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>The most appropriate Standard Industrial Classification (SIC) code for nLIGHT, Inc. based on the provided information would likely fall under the Technology sector. The specific SIC code would typically relate to the specific activities and products of the company within the technology sector. Additional details on the company's specific activities and products would be needed to precisely determine the most fitting SIC code.
+To determine the exact SIC code for nLIGHT, Inc., a more detailed analysis of the company's operations, products, and services would be necessary. This information can usually be found in the company's official filings, website, or other public documents.</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>The most appropriate NAICS code for nLIGHT, Inc, a provider of high-power semiconductor and fiber lasers for various applications, is 334510 - Electromedical and Electrotherapeutic Apparatus Manufacturing【4:2†source】.</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc's industry classification on LinkedIn is Technology【4:0†source】.</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>nLIGHT, Inc operates within the Technology sector. In addition to this classification, nLIGHT can also be categorized within the "electronic equipment" industry. Some of nLIGHT's main competitors in this industry include companies like Planet Labs PBC, Silicon Motion Technology, Himax Technologies, NextNav, Daqo New Energy, Applied Optoelectronics, JinkoSolar, Ichor, Penguin Solutions, and CommScope【4:1†source】.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AOSL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd, also known as AOS, is a designer, developer, and global supplier of a wide range of power semiconductors, including discrete power devices, wide band gap power devices, power management integrated circuits (ICs), and modules. They offer products such as Power MOSFET, SiC, IGBT, IPM, TVS, HV Gate Drivers, Power IC, and Digital Power products. AOS leverages its expertise in semiconductor process technology, product design, and packaging to develop high-performance power management solutions targeting various high-volume applications like portable computers, flat-panel TVs, LED lighting, smartphones, battery packs, consumer and industrial motor controls, and power supplies for various electronic devices. 
+The company differentiates itself by integrating its discrete and IC semiconductor technologies to address the increasingly complex power requirements of advanced electronics. AOS aims to transition from being a component supplier to becoming a comprehensive solution provider, focusing on increasing Bill of Materials (BOM) content and expanding into new products and verticals to drive growth in the future【4:0†source】【4:3†source】.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd (AOS) offers a wide range of products including discrete power devices, wide band gap power devices, power management ICs, and modules. Their portfolio includes Power MOSFET, SiC, IGBT, IPM, TVS, HV Gate Drivers, Power IC, and Digital Power products. These products target high-volume applications such as portable computers, flat-panel TVs, LED lighting, smartphones, battery packs, consumer and industrial motor controls, automotive electronics, and power supplies for various electronics like TVs, computers, servers, and telecommunications equipment【4:0†source】. AOS differentiates itself by integrating its Discrete and IC semiconductor process technology, product design, and advanced packaging expertise to provide high-performance power management solutions【4:0†source】.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd's primary target market or industry vertical includes high-volume applications such as portable computers, flat panel TVs, LED lighting, smartphones, battery packs, consumer and industrial motor controls, automotive electronics, and power supplies for various electronic devices like TVs, computers, servers, and telecommunications equipment【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd's secondary target market includes mobile applications such as smartphones, battery protection, and quick chargers. The company has successfully landed partnerships with major smartphone OEMs and ODMs, leading to significant growth in its mobile business revenue. They are focusing on expanding their presence in multiple generations of smartphone models and peripheral devices. Additionally, the company plans to leverage a joint venture company to support the demand for mobile products and aims to reach a target run rate in the near future【4:3†source】.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd's tertiary target market includes portable computers, flat panel TVs, LED lighting, smartphones, battery packs, consumer and industrial motor controls, automotive electronics, and power supplies for TVs, computers, servers, and telecommunications equipment【4:0†source】.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd serves significant markets including the aerospace and defense sector, industrial applications, and microfabrication. In the aerospace and defense market, the company has seen consistent growth over the years, supplying mission-critical lasers and actively participating in directed energy programs. In the industrial sector, particularly in China, there has been a demand for higher power laser solutions, with a focus on differentiated programmable laser technology. Additionally, in the microfabrication market, the company is catering to electronics manufacturing applications like 5G networks, flexible printed circuits, consumer electronics, medical devices, displays, and other advanced electronics applications【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>The total addressable market size for Alpha and Omega Semiconductor Ltd's primary market is estimated to be around $500 million to $600 million based on the smartphone category alone, with an average selling price range of $8 to $10 per smartphone【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>The total addressable market size for Alpha and Omega Semiconductor Ltd's secondary market is estimated to be around $500 million to $600 million, with the company aiming to capture its fair share of this market【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>The total addressable market size for Alpha and Omega Semiconductor Ltd in their tertiary market is estimated to be around $500 million to $600 million【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>The specific total addressable market size for Alpha and Omega Semiconductor Ltd's significant markets is not directly provided in the documents available. The information focuses more on financial performance, revenue breakdown by end markets like aerospace and defense, industrial end markets, microfabrication, and revenue growth trends rather than the total addressable market size for each segment【4:1†source】【4:2†source】. For a precise estimation of the total addressable market size for each significant market of Alpha and Omega Semiconductor Ltd, further market research and industry analysis specific to each segment would be necessary.</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for Alpha and Omega Semiconductor Ltd's primary market is forecasted to be around $44.114 USD after five years【4:4†source】.</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for Alpha and Omega Semiconductor Ltd's secondary market is forecasted to range from $21.15 to $51.43 in 2025【4:1†source】. This implies a significant potential return on investment of 48.05% compared to current prices.</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for Alpha and Omega Semiconductor Ltd's tertiary market is forecasted to be $44.114 USD in 5 years【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>The projected 5-year Compound Annual Growth Rate (CAGR) for Alpha and Omega Semiconductor Ltd's other markets is not explicitly provided in the available information. The data focuses more on stock price predictions and revenue growth forecasts rather than specific CAGR values for other markets【4:0†source】【4:1†source】. If you require more detailed information on the CAGR for specific markets of Alpha and Omega Semiconductor Ltd, further analysis or specific data related to those markets may be needed.</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>**Competitive Analysis of Alpha and Omega Semiconductor Ltd:**
+**Strengths:**
+1. **Integrated Technology Platform:** Alpha and Omega Semiconductor competes effectively through its integrated and innovative technology platform and design capabilities, including a multi-chip approach to power IC products.
+2. **Global Business Model:** The company benefits from a strategic global business model, allowing it to access diverse markets and customers.
+3. **Product Portfolio:** Alpha and Omega Semiconductor has an expanding portfolio of products targeting high-volume applications in various sectors such as portable computers, LED lighting, smartphones, and consumer and industrial motor controls.
+4. **Customer Base:** The company enjoys a diversified and broad customer base, reducing dependency on specific clients.
+5. **Quick Time to Market:** Alpha and Omega Semiconductor provides excellent on-the-ground support and quick time to market for its products, enhancing competitiveness in fast-moving industries【4:4†source】.
+**Weaknesses:**
+1. **Financial Resources:** Some competitors have significantly greater financial resources, which can impact Alpha and Omega Semiconductor's ability to invest in research and development, marketing, or manufacturing.
+2. **Brand Recognition:** Competitors may have more established brand recognition, potentially influencing customer preferences and market positioning.
+3. **Operating Histories:** Some competitors have longer operating histories, which could imply greater experience and credibility in the market.
+4. **Technical Resources:** Competitors might possess more advanced technical capabilities and resources, impacting the development of cutting-edge technologies and products.
+5. **Market Share:** Compared to competitors like Power Integrations, Alpha and Omega Semiconductor faces challenges in various aspects including media sentiment, analyst recommendations, earnings, and profitability【4:1†source】【4:4†source】.
+In conclusion, Alpha and Omega Semiconductor Ltd excels in technological innovation, global reach, diverse product offerings, and agile product launches. However, its weaknesses lie in areas such as financial resources, brand recognition, and competition from companies with stronger market positions. To strengthen its competitive position, the company could focus on enhancing brand awareness, investing in R&amp;D, and leveraging its existing strengths in innovation and customer relationships.</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd faces competition from companies such as Power Integrations, Ambarella, Semtech, Diodes, MaxLinear, CEVA, NVE, QuickLogic, GSI Technology, and NVIDIA in the semiconductor industry【4:1†source】. While a specific market share percentage for Alpha and Omega Semiconductor Ltd in their primary market is not explicitly provided in the documents, further market research or financial reports from the company or industry analysts may offer insights into their current estimated market share percentage.</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd's projected market share percentage in 5 years is not explicitly mentioned in the data provided. However, there is a stock price forecast indicating that the price of Alpha and Omega Semiconductor stock is expected to reach $55.16 by 2026, representing a 58.79% gain from the current value. This suggests a positive growth trajectory for the company over the next five years【4:1†source】.
+While the exact market share percentage is not specified, the projected price increase can indicate a positive market positioning and potential growth for Alpha and Omega Semiconductor Ltd in the coming years.</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd's competitive ranking among its peers is inferior to Power Integrations. Power Integrations beats Alpha and Omega Semiconductor on 14 of the 19 factors compared between the two stocks【4:0†source】.</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd competes in the semiconductor industry against companies like Power Integrations, Ambarella, Semtech, Diodes, MaxLinear, CEVA, NVE, QuickLogic, GSI Technology, and NVIDIA. While some competitors have longer operating histories, more brand recognition, and greater resources in various aspects, Alpha and Omega Semiconductor believes it can compete effectively through its integrated and innovative technology platform, design capabilities, multi-chip approach to power IC products, global business model, expanding product portfolio, diversified customer base, and quick time to market for its products【4:1†source】【4:4†source】.</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd is primarily classified in the "semiconductors" industry. Some of its main competitors in this industry include Power Integrations, Ambarella, Semtech, Diodes, MaxLinear, CEVA, NVE, QuickLogic, GSI Technology, and NVIDIA【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd operates in the "semiconductors" industry as highlighted in the information provided【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd operates in the "semiconductors" industry【4:3†source】.</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>The most appropriate SIC code for Alpha and Omega Semiconductor Ltd is likely 3674, which corresponds to "Semiconductors and Related Devices" within the Standard Industrial Classification (SIC) system【4:4†source】.</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>The most appropriate NAICS code for Alpha and Omega Semiconductor Ltd, a company specializing in power semiconductor products, would likely fall under NAICS code 334413 - Semiconductor and Related Device Manufacturing. This code specifically covers establishments primarily engaged in manufacturing semiconductors and related solid-state devices【4:2†source】.</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>Alpha and Omega Semiconductor Ltd's industry classification on LinkedIn is in the "semiconductors" industry【4:1†source】.</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>The relevant industry classifications that apply to Alpha and Omega Semiconductor Ltd include the "semiconductors" industry. Some of its main competitors in this industry are Power Integrations, Ambarella, Semtech, Diodes, MaxLinear, CEVA, NVE, QuickLogic, GSI Technology, and NVIDIA【4:0†source】.</t>
         </is>
       </c>
     </row>

</xml_diff>